<commit_message>
push for 3rd test round 1
</commit_message>
<xml_diff>
--- a/protocol.xlsx
+++ b/protocol.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\horiba-automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0BBEAD1-BBEA-4749-8C2C-E654EFE86513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A1C0F2-6288-4B14-A190-6D65267F89F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34890" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Protocol Summary</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>MESA,E02\n</t>
+  </si>
+  <si>
+    <t>usb error</t>
+  </si>
+  <si>
+    <t>MESA,E03\n</t>
   </si>
 </sst>
 </file>
@@ -414,7 +420,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,6 +496,14 @@
         <v>18</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>

</xml_diff>